<commit_message>
Build site at 2022-12-02 16:06:52 UTC
</commit_message>
<xml_diff>
--- a/assets/disciplinas/LOM3213.xlsx
+++ b/assets/disciplinas/LOM3213.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t>Ementa atual:</t>
   </si>
@@ -116,6 +116,13 @@
   </si>
   <si>
     <t>Aplicação de uma prova escrita dentro do prazo regimental antes do início do próximo semestre letivo. A nota da segunda avaliação será a média aritmética entre a nota da prova de recuperação e a nota final da primeira avaliação</t>
+  </si>
+  <si>
+    <t>Requisitos:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOM3049 -  Termodinâmica de Máquinas  (Requisito)
+</t>
   </si>
 </sst>
 </file>
@@ -471,7 +478,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -677,6 +684,19 @@
         <v>33</v>
       </c>
     </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="30" customHeight="1">
+      <c r="B23" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>